<commit_message>
Camouflages - Back + front + js checked + gold
</commit_message>
<xml_diff>
--- a/assets/xlsx/Cod4.xlsx
+++ b/assets/xlsx/Cod4.xlsx
@@ -11,7 +11,7 @@
     <sheet state="visible" name="Streak" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Map" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Campaign Mission" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Camouflages" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="Camouflage" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Weapon!$A$1:$Z$1000</definedName>
@@ -19,7 +19,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="ANPs7+AguM6YsGSzVUxXkhaQKvL8PeC59dtIlGSSLww="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataChecksum="d5zFai0fF+vEDMeQoaZwotVEjazjomzy4ifUR/glhhQ="/>
     </ext>
   </extLst>
 </workbook>
@@ -457,7 +457,7 @@
     <t>Ukraine</t>
   </si>
   <si>
-    <t>Wasteland, Bloc, Shipment, Vacant</t>
+    <t>Bloc, Shipment, Vacant</t>
   </si>
   <si>
     <t>One Shot, One Kill</t>

</xml_diff>